<commit_message>
Enable translation of Detail_Answer
</commit_message>
<xml_diff>
--- a/tests/test_translation_translate.xlsx
+++ b/tests/test_translation_translate.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamdwyer/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AD9193-CD49-9B40-862A-AD4D79987CF8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="124">
   <si>
     <t>Context</t>
   </si>
@@ -260,7 +269,7 @@
     </r>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="10"/>
         <rFont val="Calibri"/>
@@ -390,35 +399,52 @@
   <si>
     <t>Bloc 1</t>
   </si>
+  <si>
+    <t>legal_basis</t>
+  </si>
+  <si>
+    <t>Notice is given under section 1 of the Statistics of Trade Act 1947.</t>
+  </si>
+  <si>
+    <t>feeling-bad-answer</t>
+  </si>
+  <si>
+    <t>Specify why answering for yourself is bad</t>
+  </si>
+  <si>
+    <t>Nodwch pam mae ateb drosti eich hun yn wael</t>
+  </si>
+  <si>
+    <t>Rhoddir rhybudd o dan adran 1 o Ddeddf Ystadegau Masnach 1947.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color indexed="8"/>
+      <u/>
+      <sz val="11"/>
+      <color indexed="10"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <u val="single"/>
       <sz val="11"/>
-      <color indexed="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212121"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -454,23 +480,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,24 +498,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -622,7 +702,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -631,7 +711,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -640,7 +720,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -714,7 +794,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -722,7 +802,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -741,7 +821,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -771,7 +851,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -797,7 +877,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -823,7 +903,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -849,7 +929,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -875,7 +955,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -901,7 +981,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -927,7 +1007,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -953,7 +1033,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -979,7 +1059,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -992,9 +1072,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1009,7 +1095,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="38000"/>
             </a:srgbClr>
@@ -1017,7 +1103,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1036,7 +1122,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1062,7 +1148,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1088,7 +1174,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1114,7 +1200,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1140,7 +1226,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1166,7 +1252,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1192,7 +1278,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1218,7 +1304,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1244,7 +1330,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1270,7 +1356,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1283,9 +1369,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1299,7 +1391,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1318,7 +1410,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1348,7 +1440,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1374,7 +1466,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1400,7 +1492,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1426,7 +1518,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1452,7 +1544,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1478,7 +1570,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1504,7 +1596,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1530,7 +1622,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1556,7 +1648,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1569,736 +1661,772 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:IV56"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="8.85156" style="1" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="218" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="256" width="8.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="2">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s" s="2">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="2">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s" s="2">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s" s="2">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="2">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s" s="2">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s" s="2">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="2">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s" s="2">
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s" s="2">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="2">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s" s="2">
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s" s="2">
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="2">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s" s="2">
+      <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" t="s" s="2">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s" s="2">
+      <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s" s="2">
+      <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" t="s" s="2">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s" s="2">
+      <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s" s="2">
+      <c r="C9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" t="s" s="2">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s" s="2">
+      <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C10" t="s" s="2">
+      <c r="C10" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" ht="15" customHeight="1">
-      <c r="A11" t="s" s="2">
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s" s="2">
+      <c r="B11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C11" t="s" s="2">
+      <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" ht="15" customHeight="1">
-      <c r="A12" t="s" s="2">
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="s" s="2">
+      <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C12" t="s" s="2">
+      <c r="C12" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" ht="15" customHeight="1">
-      <c r="A13" t="s" s="2">
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B13" t="s" s="2">
+      <c r="B13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C13" t="s" s="2">
+      <c r="C13" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" ht="15" customHeight="1">
-      <c r="A14" t="s" s="2">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B14" t="s" s="2">
+      <c r="B14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C14" t="s" s="2">
+      <c r="C14" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" ht="15" customHeight="1">
-      <c r="A15" t="s" s="2">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B15" t="s" s="2">
+      <c r="B15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C15" t="s" s="2">
+      <c r="C15" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" ht="15" customHeight="1">
-      <c r="A16" t="s" s="2">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B16" t="s" s="2">
+      <c r="B16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C16" t="s" s="2">
+      <c r="C16" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" ht="15" customHeight="1">
-      <c r="A17" t="s" s="2">
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B17" t="s" s="2">
+      <c r="B17" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C17" t="s" s="2">
+      <c r="C17" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" ht="15" customHeight="1">
-      <c r="A18" t="s" s="2">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B18" t="s" s="2">
+      <c r="B18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C18" t="s" s="2">
+      <c r="C18" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" ht="15" customHeight="1">
-      <c r="A19" t="s" s="2">
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B19" t="s" s="2">
+      <c r="B19" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C19" t="s" s="2">
+      <c r="C19" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" ht="15" customHeight="1">
-      <c r="A20" t="s" s="2">
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B20" t="s" s="2">
+      <c r="B20" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C20" t="s" s="2">
+      <c r="C20" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" ht="15" customHeight="1">
-      <c r="A21" t="s" s="2">
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B21" t="s" s="2">
+      <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C21" t="s" s="2">
+      <c r="C21" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" ht="15" customHeight="1">
-      <c r="A22" t="s" s="2">
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B22" t="s" s="2">
+      <c r="B22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C22" t="s" s="2">
+      <c r="C22" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" ht="15" customHeight="1">
-      <c r="A23" t="s" s="2">
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B23" t="s" s="2">
+      <c r="B23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C23" t="s" s="2">
+      <c r="C23" s="2" t="s">
         <v>53</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" ht="15" customHeight="1">
-      <c r="A24" t="s" s="2">
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B24" t="s" s="2">
+      <c r="B24" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C24" t="s" s="2">
+      <c r="C24" s="2" t="s">
         <v>55</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" ht="15" customHeight="1">
-      <c r="A25" t="s" s="2">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B25" t="s" s="2">
+      <c r="B25" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C25" t="s" s="2">
+      <c r="C25" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" ht="15" customHeight="1">
-      <c r="A26" t="s" s="2">
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B26" t="s" s="2">
+      <c r="B26" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C26" t="s" s="2">
+      <c r="C26" s="2" t="s">
         <v>57</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" ht="15" customHeight="1">
-      <c r="A27" t="s" s="2">
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B27" t="s" s="2">
+      <c r="B27" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C27" t="s" s="2">
+      <c r="C27" s="2" t="s">
         <v>59</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" ht="15" customHeight="1">
-      <c r="A28" t="s" s="2">
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B28" t="s" s="2">
+      <c r="B28" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C28" t="s" s="2">
+      <c r="C28" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" ht="15" customHeight="1">
-      <c r="A29" t="s" s="2">
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B29" t="s" s="2">
+      <c r="B29" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C29" t="s" s="2">
+      <c r="C29" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" ht="15" customHeight="1">
-      <c r="A30" t="s" s="2">
+    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B30" t="s" s="2">
+      <c r="B30" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C30" t="s" s="2">
+      <c r="C30" s="2" t="s">
         <v>65</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" ht="15" customHeight="1">
-      <c r="A31" t="s" s="2">
+    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B31" t="s" s="2">
+      <c r="B31" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C31" t="s" s="2">
+      <c r="C31" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" ht="15" customHeight="1">
-      <c r="A32" t="s" s="2">
+    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B32" t="s" s="2">
+      <c r="B32" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C32" t="s" s="2">
+      <c r="C32" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" ht="15" customHeight="1">
-      <c r="A33" t="s" s="2">
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B33" t="s" s="2">
+      <c r="B33" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C33" t="s" s="2">
+      <c r="C33" s="2" t="s">
         <v>69</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
     </row>
-    <row r="34" ht="15" customHeight="1">
-      <c r="A34" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="B34" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="C34" t="s" s="2">
-        <v>72</v>
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>123</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" ht="15" customHeight="1">
-      <c r="A35" t="s" s="2">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B35" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="C35" t="s" s="2">
-        <v>74</v>
+      <c r="B35" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
     </row>
-    <row r="36" ht="15" customHeight="1">
-      <c r="A36" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="B36" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="C36" t="s" s="2">
-        <v>77</v>
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" ht="15" customHeight="1">
-      <c r="A37" t="s" s="2">
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B37" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="C37" t="s" s="2">
-        <v>79</v>
+      <c r="B37" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
     </row>
-    <row r="38" ht="15" customHeight="1">
-      <c r="A38" t="s" s="2">
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B38" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="C38" t="s" s="2">
-        <v>81</v>
+      <c r="B38" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" ht="15" customHeight="1">
-      <c r="A39" t="s" s="2">
+    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B39" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="C39" t="s" s="2">
-        <v>83</v>
+      <c r="B39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
     </row>
-    <row r="40" ht="15" customHeight="1">
-      <c r="A40" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="B40" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="C40" t="s" s="2">
-        <v>86</v>
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" ht="15" customHeight="1">
-      <c r="A41" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="B41" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="C41" t="s" s="2">
-        <v>88</v>
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>122</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" ht="15" customHeight="1">
-      <c r="A42" t="s" s="2">
+    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B42" t="s" s="2">
-        <v>89</v>
-      </c>
-      <c r="C42" t="s" s="2">
-        <v>90</v>
+      <c r="B42" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" ht="15" customHeight="1">
-      <c r="A43" t="s" s="2">
+    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B43" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="C43" t="s" s="2">
-        <v>92</v>
+      <c r="B43" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
     </row>
-    <row r="44" ht="15" customHeight="1">
-      <c r="A44" t="s" s="2">
-        <v>93</v>
-      </c>
-      <c r="B44" t="s" s="2">
-        <v>94</v>
-      </c>
-      <c r="C44" t="s" s="2">
-        <v>95</v>
+    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
     </row>
-    <row r="45" ht="15" customHeight="1">
-      <c r="A45" t="s" s="2">
-        <v>93</v>
-      </c>
-      <c r="B45" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="C45" t="s" s="2">
-        <v>97</v>
+    <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
     </row>
-    <row r="46" ht="15" customHeight="1">
-      <c r="A46" t="s" s="2">
+    <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B46" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="C46" t="s" s="2">
-        <v>88</v>
+      <c r="B46" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
     </row>
-    <row r="47" ht="15" customHeight="1">
-      <c r="A47" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="B47" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="C47" t="s" s="2">
-        <v>99</v>
+    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" ht="15" customHeight="1">
-      <c r="A48" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="B48" t="s" s="2">
-        <v>101</v>
-      </c>
-      <c r="C48" t="s" s="2">
-        <v>102</v>
+    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
     </row>
-    <row r="49" ht="15" customHeight="1">
-      <c r="A49" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="B49" t="s" s="2">
-        <v>103</v>
-      </c>
-      <c r="C49" t="s" s="2">
-        <v>104</v>
+    <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
     </row>
-    <row r="50" ht="15" customHeight="1">
-      <c r="A50" t="s" s="2">
+    <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B50" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="C50" t="s" s="2">
-        <v>106</v>
+      <c r="B50" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
     </row>
-    <row r="51" ht="15" customHeight="1">
-      <c r="A51" t="s" s="2">
-        <v>107</v>
-      </c>
-      <c r="B51" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="C51" t="s" s="2">
-        <v>109</v>
+    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
     </row>
-    <row r="52" ht="15" customHeight="1">
-      <c r="A52" t="s" s="2">
-        <v>107</v>
-      </c>
-      <c r="B52" t="s" s="2">
-        <v>110</v>
-      </c>
-      <c r="C52" t="s" s="2">
-        <v>111</v>
+    <row r="52" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
     </row>
-    <row r="53" ht="15" customHeight="1">
-      <c r="A53" t="s" s="2">
-        <v>112</v>
-      </c>
-      <c r="B53" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="C53" t="s" s="2">
-        <v>114</v>
+    <row r="53" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
     </row>
-    <row r="54" ht="15" customHeight="1">
-      <c r="A54" t="s" s="2">
-        <v>115</v>
-      </c>
-      <c r="B54" t="s" s="2">
-        <v>116</v>
-      </c>
-      <c r="C54" t="s" s="2">
-        <v>117</v>
+    <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
     </row>
+    <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C37" r:id="rId1" location="" tooltip="" display=""/>
+    <hyperlink ref="C38" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>